<commit_message>
Finish data population script
</commit_message>
<xml_diff>
--- a/population_script/data.xlsx
+++ b/population_script/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinwoods/Documents/GitHub/Paper_Archive_Maintenance_Activity/population_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D52E26F-F76C-2646-956B-12430DAD4D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D7E734-3F75-4444-B85C-D6EB7859515D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2200" yWindow="500" windowWidth="28040" windowHeight="14940" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="14940" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Unstructured Text</t>
   </si>
   <si>
-    <t>NLP Identified item</t>
-  </si>
-  <si>
     <t>Work Order Type</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
   </si>
   <si>
     <t>NLP Identified Activity</t>
+  </si>
+  <si>
+    <t>NLP Identified Item</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,22 +710,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -733,22 +733,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H2" s="2">
         <v>560.96</v>
@@ -762,22 +762,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" s="2">
         <v>1292.1300000000001</v>
@@ -791,22 +791,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4" s="2">
         <v>413.48</v>
@@ -820,22 +820,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" s="2">
         <v>516.85</v>
@@ -849,22 +849,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H6" s="2">
         <v>560.96</v>
@@ -878,22 +878,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -907,22 +907,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="2">
         <v>258.43</v>
@@ -936,22 +936,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="2">
         <v>322.26</v>
@@ -965,22 +965,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H10" s="2">
         <v>400.31</v>
@@ -994,22 +994,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H11" s="2">
         <v>413.48</v>
@@ -1023,22 +1023,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="2">
         <v>650.6</v>
@@ -1052,22 +1052,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
@@ -1081,22 +1081,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H14" s="2">
         <v>3195.48</v>
@@ -1110,22 +1110,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" s="2">
         <v>680.81</v>
@@ -1139,22 +1139,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H16" s="2">
         <v>145.34</v>
@@ -1168,22 +1168,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H17" s="2">
         <v>64</v>
@@ -1197,22 +1197,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H18" s="2">
         <v>400.31</v>
@@ -1226,22 +1226,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H19" s="2">
         <v>131.4</v>
@@ -1255,22 +1255,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1284,22 +1284,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H21" s="2">
         <v>82.38</v>
@@ -1313,22 +1313,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H22" s="2">
         <v>348.71</v>
@@ -1342,22 +1342,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H23" s="2">
         <v>270.85000000000002</v>
@@ -1371,22 +1371,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H24" s="2">
         <v>541.69000000000005</v>
@@ -1400,22 +1400,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H25" s="2">
         <v>322.92</v>
@@ -1429,22 +1429,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H26" s="2">
         <v>478.77</v>
@@ -1458,22 +1458,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H27" s="2">
         <v>91.18</v>
@@ -1487,22 +1487,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H28" s="2">
         <v>5168.6000000000004</v>
@@ -1516,22 +1516,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H29" s="2">
         <v>868.73</v>
@@ -1545,22 +1545,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H30" s="2">
         <v>601.07000000000005</v>
@@ -1574,22 +1574,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H31" s="2">
         <v>8632.82</v>
@@ -1603,22 +1603,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H32" s="2">
         <v>282.81</v>
@@ -1632,22 +1632,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H33" s="2">
         <v>726.03</v>
@@ -1661,22 +1661,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
         <v>75</v>
       </c>
-      <c r="E34" t="s">
-        <v>76</v>
-      </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H34" s="2">
         <v>269.2</v>
@@ -1690,22 +1690,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H35" s="2">
         <v>3207.65</v>
@@ -1719,22 +1719,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" t="s">
         <v>68</v>
       </c>
-      <c r="D36" t="s">
-        <v>69</v>
-      </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H36" s="2">
         <v>99.36</v>
@@ -1748,22 +1748,22 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H37" s="2">
         <v>198.72</v>

</xml_diff>

<commit_message>
Update data file to include ground truth from logic tree
</commit_message>
<xml_diff>
--- a/population_script/data.xlsx
+++ b/population_script/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinwoods/Documents/GitHub/Paper_Archive_Maintenance_Activity/population_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D7E734-3F75-4444-B85C-D6EB7859515D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBD26F6-3D86-F146-8164-3E1C7A67983C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="14940" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
+    <workbookView xWindow="33600" yWindow="-1520" windowWidth="28040" windowHeight="18860" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$37</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -174,9 +175,6 @@
     <t>calibrate pressure switch</t>
   </si>
   <si>
-    <t>pump not pumping wekk</t>
-  </si>
-  <si>
     <t>pressure switch leaking</t>
   </si>
   <si>
@@ -322,6 +320,24 @@
   </si>
   <si>
     <t>NLP Identified Item</t>
+  </si>
+  <si>
+    <t>Correct Class (from logic tree)</t>
+  </si>
+  <si>
+    <t>repair/replace</t>
+  </si>
+  <si>
+    <t>adjust/ calibrate</t>
+  </si>
+  <si>
+    <t>repair/ replace</t>
+  </si>
+  <si>
+    <t>Work not actioned</t>
+  </si>
+  <si>
+    <t>pump not pumping well</t>
   </si>
 </sst>
 </file>
@@ -337,7 +353,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +363,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,10 +385,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD16A520-B3EA-B04E-B228-230F864C4781}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,9 +720,10 @@
     <col min="7" max="7" width="18.83203125" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,13 +734,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -727,8 +751,11 @@
       <c r="I1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -739,16 +766,16 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="2">
         <v>560.96</v>
@@ -756,8 +783,11 @@
       <c r="I2" s="2">
         <v>821.74</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -768,16 +798,16 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H3" s="2">
         <v>1292.1300000000001</v>
@@ -785,8 +815,11 @@
       <c r="I3" s="2">
         <v>711.11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -797,16 +830,16 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="2">
         <v>413.48</v>
@@ -814,8 +847,11 @@
       <c r="I4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -823,19 +859,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" s="2">
         <v>516.85</v>
@@ -843,8 +879,11 @@
       <c r="I5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -852,19 +891,19 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H6" s="2">
         <v>560.96</v>
@@ -872,8 +911,11 @@
       <c r="I6" s="2">
         <v>700</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -884,16 +926,16 @@
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -901,8 +943,11 @@
       <c r="I7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -910,19 +955,19 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8" s="2">
         <v>258.43</v>
@@ -930,8 +975,11 @@
       <c r="I8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -942,16 +990,16 @@
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="2">
         <v>322.26</v>
@@ -959,8 +1007,11 @@
       <c r="I9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -971,16 +1022,16 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H10" s="2">
         <v>400.31</v>
@@ -988,8 +1039,11 @@
       <c r="I10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1000,16 +1054,16 @@
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" s="2">
         <v>413.48</v>
@@ -1017,8 +1071,11 @@
       <c r="I11" s="2">
         <v>1455</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1026,19 +1083,19 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" s="2">
         <v>650.6</v>
@@ -1046,8 +1103,11 @@
       <c r="I12" s="2">
         <v>344.52</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1055,19 +1115,19 @@
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
@@ -1075,8 +1135,11 @@
       <c r="I13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1084,19 +1147,19 @@
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H14" s="2">
         <v>3195.48</v>
@@ -1104,8 +1167,11 @@
       <c r="I14" s="2">
         <v>5062.28</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1113,19 +1179,19 @@
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15" s="2">
         <v>680.81</v>
@@ -1133,8 +1199,11 @@
       <c r="I15" s="2">
         <v>1133.1300000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1142,19 +1211,19 @@
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H16" s="2">
         <v>145.34</v>
@@ -1162,8 +1231,11 @@
       <c r="I16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1171,19 +1243,19 @@
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
         <v>64</v>
@@ -1191,8 +1263,11 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1200,19 +1275,19 @@
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" s="2">
         <v>400.31</v>
@@ -1220,8 +1295,11 @@
       <c r="I18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1229,19 +1307,19 @@
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H19" s="2">
         <v>131.4</v>
@@ -1249,8 +1327,11 @@
       <c r="I19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1258,19 +1339,19 @@
         <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1278,8 +1359,11 @@
       <c r="I20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1287,19 +1371,19 @@
         <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H21" s="2">
         <v>82.38</v>
@@ -1307,8 +1391,11 @@
       <c r="I21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1316,19 +1403,19 @@
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H22" s="2">
         <v>348.71</v>
@@ -1336,8 +1423,11 @@
       <c r="I22" s="2">
         <v>1200</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1345,19 +1435,19 @@
         <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H23" s="2">
         <v>270.85000000000002</v>
@@ -1365,8 +1455,11 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1377,16 +1470,16 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H24" s="2">
         <v>541.69000000000005</v>
@@ -1394,8 +1487,11 @@
       <c r="I24" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1403,19 +1499,19 @@
         <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H25" s="2">
         <v>322.92</v>
@@ -1423,8 +1519,11 @@
       <c r="I25" s="2">
         <v>110.59</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1432,19 +1531,19 @@
         <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H26" s="2">
         <v>478.77</v>
@@ -1452,8 +1551,11 @@
       <c r="I26" s="2">
         <v>110.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1461,19 +1563,19 @@
         <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H27" s="2">
         <v>91.18</v>
@@ -1481,8 +1583,11 @@
       <c r="I27" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1490,19 +1595,19 @@
         <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H28" s="2">
         <v>5168.6000000000004</v>
@@ -1510,8 +1615,11 @@
       <c r="I28" s="2">
         <v>15370.28</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1519,19 +1627,19 @@
         <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H29" s="2">
         <v>868.73</v>
@@ -1539,8 +1647,11 @@
       <c r="I29" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1548,19 +1659,19 @@
         <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H30" s="2">
         <v>601.07000000000005</v>
@@ -1568,8 +1679,11 @@
       <c r="I30" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1577,19 +1691,19 @@
         <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H31" s="2">
         <v>8632.82</v>
@@ -1597,8 +1711,11 @@
       <c r="I31" s="2">
         <v>8369.93</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1606,19 +1723,19 @@
         <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H32" s="2">
         <v>282.81</v>
@@ -1626,8 +1743,11 @@
       <c r="I32" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1635,19 +1755,19 @@
         <v>36</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H33" s="2">
         <v>726.03</v>
@@ -1655,8 +1775,11 @@
       <c r="I33" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1664,19 +1787,19 @@
         <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" t="s">
         <v>74</v>
       </c>
-      <c r="E34" t="s">
-        <v>75</v>
-      </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H34" s="2">
         <v>269.2</v>
@@ -1684,8 +1807,11 @@
       <c r="I34" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1693,19 +1819,19 @@
         <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H35" s="2">
         <v>3207.65</v>
@@ -1713,8 +1839,11 @@
       <c r="I35" s="2">
         <v>566.66</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1722,19 +1851,19 @@
         <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
         <v>67</v>
       </c>
-      <c r="D36" t="s">
-        <v>68</v>
-      </c>
       <c r="E36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H36" s="2">
         <v>99.36</v>
@@ -1742,8 +1871,11 @@
       <c r="I36" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1751,25 +1883,28 @@
         <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H37" s="2">
         <v>198.72</v>
       </c>
       <c r="I37" s="2">
         <v>2021</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix / tweak script - added Pump Unit System (and punned individual)
</commit_message>
<xml_diff>
--- a/population_script/data.xlsx
+++ b/population_script/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinwoods/Documents/GitHub/Paper_Archive_Maintenance_Activity/population_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBD26F6-3D86-F146-8164-3E1C7A67983C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E72865-BF1B-1847-B855-85BDF21DD00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-1520" windowWidth="28040" windowHeight="18860" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
+    <workbookView xWindow="8400" yWindow="500" windowWidth="20400" windowHeight="16340" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>piping and valves</t>
   </si>
   <si>
-    <t>lubrication system</t>
-  </si>
-  <si>
     <t>preventative</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>pump not pumping well</t>
+  </si>
+  <si>
+    <t>lubrication</t>
   </si>
 </sst>
 </file>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD16A520-B3EA-B04E-B228-230F864C4781}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,10 +734,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
         <v>84</v>
@@ -752,7 +752,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -784,7 +784,7 @@
         <v>821.74</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>711.11</v>
       </c>
       <c r="J3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
         <v>68</v>
@@ -880,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
         <v>700</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -967,7 +967,7 @@
         <v>88</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="2">
         <v>258.43</v>
@@ -1008,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1072,7 +1072,7 @@
         <v>1455</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
         <v>344.52</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1124,7 +1124,7 @@
         <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>85</v>
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1168,7 +1168,7 @@
         <v>5062.28</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1200,7 +1200,7 @@
         <v>1133.1300000000001</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1319,7 +1319,7 @@
         <v>88</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H19" s="2">
         <v>131.4</v>
@@ -1351,7 +1351,7 @@
         <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1360,7 +1360,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1424,7 +1424,7 @@
         <v>1200</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1456,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1511,7 +1511,7 @@
         <v>87</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H25" s="2">
         <v>322.92</v>
@@ -1543,7 +1543,7 @@
         <v>87</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H26" s="2">
         <v>478.77</v>
@@ -1575,7 +1575,7 @@
         <v>88</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H27" s="2">
         <v>91.18</v>
@@ -1616,7 +1616,7 @@
         <v>15370.28</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1639,7 +1639,7 @@
         <v>88</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H29" s="2">
         <v>868.73</v>
@@ -1668,7 +1668,7 @@
         <v>83</v>
       </c>
       <c r="F30" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>85</v>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1703,7 +1703,7 @@
         <v>87</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H31" s="2">
         <v>8632.82</v>
@@ -1712,7 +1712,7 @@
         <v>8369.93</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1744,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -1767,7 +1767,7 @@
         <v>88</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H33" s="2">
         <v>726.03</v>
@@ -1808,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -1840,7 +1840,7 @@
         <v>566.66</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -1872,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -1904,7 +1904,7 @@
         <v>2021</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to commit corrections to decision tree results
</commit_message>
<xml_diff>
--- a/population_script/data.xlsx
+++ b/population_script/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinwoods/Documents/GitHub/Paper_Archive_Maintenance_Activity/population_script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Research\projects\OGI Pilot-OIIE\IOF Maintenance Working Group Meetings\paper_related_ontology_repos\AppliedOntology_Maintenance_Activities\population_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E72865-BF1B-1847-B855-85BDF21DD00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B64F2-4474-4413-AEB8-DEAD3C7A0756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="500" windowWidth="20400" windowHeight="16340" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
+    <workbookView xWindow="1080" yWindow="-120" windowWidth="27840" windowHeight="18240" xr2:uid="{BEFAB777-0333-6541-9FEF-E59293AC42EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>lubrication</t>
+  </si>
+  <si>
+    <t>diagnose</t>
   </si>
 </sst>
 </file>
@@ -706,24 +709,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD16A520-B3EA-B04E-B228-230F864C4781}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="26.625" customWidth="1"/>
+    <col min="6" max="6" width="27.375" customWidth="1"/>
+    <col min="7" max="7" width="18.875" customWidth="1"/>
+    <col min="8" max="8" width="20.375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="26.83203125" customWidth="1"/>
+    <col min="10" max="10" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +761,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -787,7 +793,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -819,7 +825,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -851,7 +857,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -880,10 +886,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -915,7 +921,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -947,7 +953,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -979,7 +985,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1171,7 +1177,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1203,7 +1209,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1235,7 +1241,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1264,10 +1270,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1331,7 +1337,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1392,10 +1398,10 @@
         <v>0</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1456,10 +1462,10 @@
         <v>0</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1491,7 +1497,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1523,7 +1529,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1683,7 +1689,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1712,10 +1718,10 @@
         <v>8369.93</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1744,10 +1750,10 @@
         <v>0</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1808,10 +1814,10 @@
         <v>0</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1872,10 +1878,10 @@
         <v>0</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>

</xml_diff>